<commit_message>
adicionado o banco de dados!
</commit_message>
<xml_diff>
--- a/MapaMental.xlsx
+++ b/MapaMental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suporte\Documents\Felipe Mota\projetoInsta\instagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F11EB31-AAE2-4667-8753-DE11F33C369C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE39449-5961-4B3A-9908-8AC67D6931BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18120" yWindow="4260" windowWidth="11535" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>nome</t>
   </si>
@@ -87,9 +87,6 @@
     <t>likes</t>
   </si>
   <si>
-    <t>coments</t>
-  </si>
-  <si>
     <t>lalalalala</t>
   </si>
   <si>
@@ -114,12 +111,6 @@
     <t>usuário</t>
   </si>
   <si>
-    <t>lalalalalla</t>
-  </si>
-  <si>
-    <t>SFASGFf</t>
-  </si>
-  <si>
     <t>destina</t>
   </si>
   <si>
@@ -139,13 +130,52 @@
   </si>
   <si>
     <t>ethtew</t>
+  </si>
+  <si>
+    <t>descrit</t>
+  </si>
+  <si>
+    <t>blabla</t>
+  </si>
+  <si>
+    <t>bleble</t>
+  </si>
+  <si>
+    <t>wow!</t>
+  </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Criador</t>
+  </si>
+  <si>
+    <t>Comentário</t>
+  </si>
+  <si>
+    <t>ttwertgWE</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>SDFSDG</t>
+  </si>
+  <si>
+    <t>3t4</t>
+  </si>
+  <si>
+    <t>sgsgsetsgysetg</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,8 +199,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,43 +252,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -280,12 +305,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -569,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,15 +633,17 @@
       <c r="L2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="5"/>
+      <c r="N2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="P2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="R2" s="7" t="s">
         <v>16</v>
@@ -655,23 +681,22 @@
         <v>2</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3">
+      <c r="N3" s="2">
         <v>1</v>
       </c>
-      <c r="O3" s="5"/>
+      <c r="O3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R3" s="2">
         <v>2</v>
@@ -709,21 +734,26 @@
         <v>1</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-      <c r="O4" s="5"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="L4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
@@ -733,141 +763,333 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="O5" s="5"/>
+      <c r="R5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="8"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2">
+        <v>5</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N9" s="2">
+        <v>2</v>
+      </c>
+      <c r="O9" s="2">
+        <v>6</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N10" s="2">
+        <v>3</v>
+      </c>
+      <c r="O10" s="2">
+        <v>7</v>
+      </c>
+      <c r="P10" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N11" s="2">
+        <v>4</v>
+      </c>
+      <c r="O11" s="2">
+        <v>8</v>
+      </c>
+      <c r="P11" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N12" s="2">
+        <v>5</v>
+      </c>
+      <c r="O12" s="2">
+        <v>9</v>
+      </c>
+      <c r="P12" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="2"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="L15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="I16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F21" s="5"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="5"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F22" s="10"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
       <c r="K23" s="5"/>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F24" s="8"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="11"/>
-      <c r="H24" s="8"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G26" s="8"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G27" s="8"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="8"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="8"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E31" s="8"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="8"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="8"/>
-    </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="8"/>
-    </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="8"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="8"/>
-    </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-    </row>
-    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F36" s="8"/>
-      <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F37" s="8"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="F38" s="10"/>
-      <c r="H38" s="10"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -895,51 +1117,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCB17C0-B0BE-4991-BB30-B06F5104B880}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H12" sqref="H12:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
         <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -949,31 +1162,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE46806-D826-4DF7-AFD8-9CAB01D429E3}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>31</v>
+      <c r="A2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,7 +1200,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1001,7 +1214,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1015,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1029,8 +1242,11 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>